<commit_message>
add () to WBC
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fumiya/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fumiya/programming/medicaltest-to-text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC17B8B-9BA1-9F46-B432-241866433A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30905AF3-F6F8-974A-9374-C5466269AAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22940" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34440" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="シート1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>赤血球</t>
   </si>
   <si>
-    <t>万</t>
-  </si>
-  <si>
     <t>Hb</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>血小板</t>
   </si>
   <si>
-    <t>✕10^4</t>
-  </si>
-  <si>
     <t>MPV</t>
   </si>
   <si>
@@ -160,12 +154,6 @@
     <t>クレアチニン</t>
   </si>
   <si>
-    <t>成人eGFR(1.73)</t>
-  </si>
-  <si>
-    <t>mL/min</t>
-  </si>
-  <si>
     <t>尿酸</t>
   </si>
   <si>
@@ -301,9 +289,6 @@
     <t>沈渣尿量</t>
   </si>
   <si>
-    <t>/HPF</t>
-  </si>
-  <si>
     <t>扁平上皮</t>
   </si>
   <si>
@@ -347,15 +332,6 @@
   </si>
   <si>
     <t>IgG[尿]</t>
-  </si>
-  <si>
-    <t>トランスフェリン[尿]</t>
-  </si>
-  <si>
-    <t>U-TF</t>
-  </si>
-  <si>
-    <t>U-TF換算</t>
   </si>
   <si>
     <t>mg/g・Cre</t>
@@ -435,6 +411,41 @@
   </si>
   <si>
     <t>総蛋白</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>万/μL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/μL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>個/HPF</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">コ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>トランスフェリン[尿]（U-TF）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>トランスフェリン[尿]（U-TF換算）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mg/dL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mL/min/1.73m^2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eGFR</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1799,7 +1810,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1810,8 +1821,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="22" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="2" customWidth="1"/>
     <col min="3" max="4" width="19.5703125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="19.5703125" style="2"/>
   </cols>
@@ -1840,131 +1851,133 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="22" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="22" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="22" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="22" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="22" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="22" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="22" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="22" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="22" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="22" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" customHeight="1">
@@ -1974,41 +1987,41 @@
     </row>
     <row r="19" spans="1:3" ht="22" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="22" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="22" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" ht="22" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="22" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="22" customHeight="1">
@@ -2018,294 +2031,294 @@
     </row>
     <row r="25" spans="1:3" ht="22" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" ht="22" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="22" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="22" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" ht="22" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="22" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="22" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="22" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="22" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="22" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="22" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="22" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="22" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="22" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="22" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" ht="22" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="22" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="22" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="22" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="22" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="22" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="22" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="22" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="22" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="22" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="22" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="22" customHeight="1">
       <c r="A54" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="22" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="22" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="22" customHeight="1">
       <c r="A57" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="22" customHeight="1">
       <c r="A58" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="9"/>
@@ -2317,27 +2330,27 @@
     </row>
     <row r="60" spans="1:3" ht="22" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" ht="22" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="22" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="22" customHeight="1">
@@ -2347,27 +2360,27 @@
     </row>
     <row r="64" spans="1:3" ht="22" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" ht="22" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="22" customHeight="1">
       <c r="A66" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="22" customHeight="1">
@@ -2377,98 +2390,98 @@
     </row>
     <row r="68" spans="1:3" ht="22" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" ht="22" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:3" ht="22" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" ht="22" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" ht="22" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" ht="22" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" ht="22" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" ht="22" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="22" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="22" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="22" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" ht="22" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="22" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" ht="22" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
@@ -2479,25 +2492,25 @@
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="8" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="22" customHeight="1">
       <c r="A83" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="8" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="22" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="8" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="22" customHeight="1">
@@ -2507,343 +2520,341 @@
     </row>
     <row r="86" spans="1:3" ht="22" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="22" customHeight="1">
       <c r="A87" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="22" customHeight="1">
       <c r="A88" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="22" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="22" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="22" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="22" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="22" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="22" customHeight="1">
       <c r="A94" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="22" customHeight="1">
       <c r="A95" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="22" customHeight="1">
       <c r="A96" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="22" customHeight="1">
       <c r="A97" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="22" customHeight="1">
       <c r="A98" s="6" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B98" s="7"/>
-      <c r="C98" s="9"/>
+      <c r="C98" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="99" spans="1:3" ht="22" customHeight="1">
       <c r="A99" s="6" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="8" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="22" customHeight="1">
-      <c r="A100" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="A100" s="10"/>
       <c r="B100" s="7"/>
-      <c r="C100" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" ht="22" customHeight="1">
-      <c r="A101" s="10"/>
+      <c r="A101" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" ht="22" customHeight="1">
       <c r="A102" s="6" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B102" s="7"/>
-      <c r="C102" s="9"/>
+      <c r="C102" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="22" customHeight="1">
       <c r="A103" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="22" customHeight="1">
       <c r="A104" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="22" customHeight="1">
       <c r="A105" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="22" customHeight="1">
       <c r="A106" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="22" customHeight="1">
       <c r="A107" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="8" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="22" customHeight="1">
-      <c r="A108" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="A108" s="10"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="8" t="s">
-        <v>119</v>
-      </c>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" ht="22" customHeight="1">
-      <c r="A109" s="10"/>
+      <c r="A109" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="B109" s="7"/>
       <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" ht="22" customHeight="1">
       <c r="A110" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B110" s="7"/>
-      <c r="C110" s="9"/>
+      <c r="C110" s="8" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="22" customHeight="1">
       <c r="A111" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B111" s="7"/>
       <c r="C111" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="22" customHeight="1">
-      <c r="A112" s="6" t="s">
-        <v>123</v>
-      </c>
+      <c r="A112" s="10"/>
       <c r="B112" s="7"/>
-      <c r="C112" s="8" t="s">
-        <v>122</v>
-      </c>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" ht="22" customHeight="1">
-      <c r="A113" s="10"/>
+      <c r="A113" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="B113" s="7"/>
       <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" ht="22" customHeight="1">
       <c r="A114" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B114" s="7"/>
-      <c r="C114" s="9"/>
+      <c r="C114" s="8" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="115" spans="1:3" ht="22" customHeight="1">
-      <c r="A115" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="A115" s="10"/>
       <c r="B115" s="7"/>
-      <c r="C115" s="8" t="s">
-        <v>122</v>
-      </c>
+      <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" ht="22" customHeight="1">
-      <c r="A116" s="10"/>
+      <c r="A116" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="B116" s="7"/>
       <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" ht="22" customHeight="1">
       <c r="A117" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B117" s="7"/>
-      <c r="C117" s="9"/>
+      <c r="C117" s="8" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="118" spans="1:3" ht="22" customHeight="1">
       <c r="A118" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B118" s="7"/>
       <c r="C118" s="8" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="22" customHeight="1">
-      <c r="A119" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="A119" s="10"/>
       <c r="B119" s="7"/>
-      <c r="C119" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" ht="22" customHeight="1">
-      <c r="A120" s="10"/>
+      <c r="A120" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="B120" s="7"/>
       <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" ht="22" customHeight="1">
       <c r="A121" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B121" s="7"/>
-      <c r="C121" s="9"/>
+      <c r="C121" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="22" customHeight="1">
-      <c r="A122" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="A122" s="10"/>
       <c r="B122" s="7"/>
-      <c r="C122" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" ht="22" customHeight="1">
-      <c r="A123" s="10"/>
+      <c r="A123" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="B123" s="7"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" ht="22" customHeight="1">
       <c r="A124" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B124" s="7"/>
-      <c r="C124" s="9"/>
+      <c r="C124" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="125" spans="1:3" ht="22" customHeight="1">
       <c r="A125" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B125" s="7"/>
       <c r="C125" s="8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="22" customHeight="1">
       <c r="A126" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B126" s="7"/>
       <c r="C126" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="22" customHeight="1">
-      <c r="A127" s="6" t="s">
-        <v>135</v>
-      </c>
+      <c r="A127" s="10"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="8" t="s">
-        <v>75</v>
-      </c>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" ht="22" customHeight="1">
       <c r="A128" s="10"/>
@@ -2994,11 +3005,6 @@
       <c r="A157" s="10"/>
       <c r="B157" s="7"/>
       <c r="C157" s="9"/>
-    </row>
-    <row r="158" spans="1:3" ht="22" customHeight="1">
-      <c r="A158" s="10"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add PT in template.xlsx
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fumiya/programming/medicaltest-to-text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5189EEEA-7952-7D4A-8FBE-61FF9D52AA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD615F1-1F60-9D4D-B7A4-279AAB5106CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="シート1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
   <si>
     <t>検査項目</t>
   </si>
@@ -469,6 +469,14 @@
     <rPh sb="7" eb="10">
       <t xml:space="preserve">ジュヨウタイ </t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sec</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1833,7 +1841,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C159"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2017,21 +2025,23 @@
     </row>
     <row r="20" spans="1:3" ht="22" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="22" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" ht="22" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
@@ -2040,7 +2050,7 @@
     </row>
     <row r="23" spans="1:3" ht="22" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
@@ -2048,41 +2058,41 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="22" customHeight="1">
-      <c r="A24" s="10"/>
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" ht="22" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="A25" s="10"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" ht="22" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="22" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="22" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" ht="22" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
@@ -2091,7 +2101,7 @@
     </row>
     <row r="30" spans="1:3" ht="22" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
@@ -2100,7 +2110,7 @@
     </row>
     <row r="31" spans="1:3" ht="22" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8" t="s">
@@ -2109,7 +2119,7 @@
     </row>
     <row r="32" spans="1:3" ht="22" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
@@ -2118,7 +2128,7 @@
     </row>
     <row r="33" spans="1:3" ht="22" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
@@ -2127,7 +2137,7 @@
     </row>
     <row r="34" spans="1:3" ht="22" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
@@ -2136,7 +2146,7 @@
     </row>
     <row r="35" spans="1:3" ht="22" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
@@ -2145,7 +2155,7 @@
     </row>
     <row r="36" spans="1:3" ht="22" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
@@ -2154,7 +2164,7 @@
     </row>
     <row r="37" spans="1:3" ht="22" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
@@ -2163,7 +2173,7 @@
     </row>
     <row r="38" spans="1:3" ht="22" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
@@ -2172,7 +2182,7 @@
     </row>
     <row r="39" spans="1:3" ht="22" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
@@ -2181,7 +2191,7 @@
     </row>
     <row r="40" spans="1:3" ht="22" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
@@ -2190,7 +2200,7 @@
     </row>
     <row r="41" spans="1:3" ht="22" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
@@ -2199,14 +2209,14 @@
     </row>
     <row r="42" spans="1:3" ht="22" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" ht="22" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
@@ -2215,7 +2225,7 @@
     </row>
     <row r="44" spans="1:3" ht="22" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
@@ -2224,7 +2234,7 @@
     </row>
     <row r="45" spans="1:3" ht="22" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="8" t="s">
@@ -2233,7 +2243,7 @@
     </row>
     <row r="46" spans="1:3" ht="22" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="8" t="s">
@@ -2242,7 +2252,7 @@
     </row>
     <row r="47" spans="1:3" ht="22" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8" t="s">
@@ -2251,7 +2261,7 @@
     </row>
     <row r="48" spans="1:3" ht="22" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>134</v>
+        <v>50</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="8" t="s">
@@ -2260,7 +2270,7 @@
     </row>
     <row r="49" spans="1:3" ht="22" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8" t="s">
@@ -2269,7 +2279,7 @@
     </row>
     <row r="50" spans="1:3" ht="22" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8" t="s">
@@ -2278,7 +2288,7 @@
     </row>
     <row r="51" spans="1:3" ht="22" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
@@ -2287,7 +2297,7 @@
     </row>
     <row r="52" spans="1:3" ht="22" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
@@ -2296,7 +2306,7 @@
     </row>
     <row r="53" spans="1:3" ht="22" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8" t="s">
@@ -2305,7 +2315,7 @@
     </row>
     <row r="54" spans="1:3" ht="22" customHeight="1">
       <c r="A54" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="8" t="s">
@@ -2314,7 +2324,7 @@
     </row>
     <row r="55" spans="1:3" ht="22" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="8" t="s">
@@ -2323,7 +2333,7 @@
     </row>
     <row r="56" spans="1:3" ht="22" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
@@ -2332,7 +2342,7 @@
     </row>
     <row r="57" spans="1:3" ht="22" customHeight="1">
       <c r="A57" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
@@ -2341,7 +2351,7 @@
     </row>
     <row r="58" spans="1:3" ht="22" customHeight="1">
       <c r="A58" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="8" t="s">
@@ -2350,7 +2360,7 @@
     </row>
     <row r="59" spans="1:3" ht="22" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="8" t="s">
@@ -2359,26 +2369,26 @@
     </row>
     <row r="60" spans="1:3" ht="22" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" ht="22" customHeight="1">
-      <c r="A61" s="10"/>
+      <c r="A61" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="B61" s="7"/>
       <c r="C61" s="9"/>
     </row>
     <row r="62" spans="1:3" ht="22" customHeight="1">
-      <c r="A62" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="A62" s="10"/>
       <c r="B62" s="7"/>
       <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" ht="22" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="8" t="s">
@@ -2387,7 +2397,7 @@
     </row>
     <row r="64" spans="1:3" ht="22" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="8" t="s">
@@ -2395,20 +2405,20 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="22" customHeight="1">
-      <c r="A65" s="10"/>
+      <c r="A65" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="B65" s="7"/>
       <c r="C65" s="9"/>
     </row>
     <row r="66" spans="1:3" ht="22" customHeight="1">
-      <c r="A66" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="A66" s="10"/>
       <c r="B66" s="7"/>
       <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" ht="22" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="8" t="s">
@@ -2417,7 +2427,7 @@
     </row>
     <row r="68" spans="1:3" ht="22" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="8" t="s">
@@ -2425,111 +2435,111 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="22" customHeight="1">
-      <c r="A69" s="10"/>
+      <c r="A69" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="B69" s="7"/>
       <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:3" ht="22" customHeight="1">
-      <c r="A70" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="A70" s="10"/>
       <c r="B70" s="7"/>
       <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" ht="22" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" ht="22" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" ht="22" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" ht="22" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" ht="22" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="22" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="22" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="22" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" ht="22" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="22" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" ht="22" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" ht="22" customHeight="1">
       <c r="A82" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" ht="22" customHeight="1">
       <c r="A83" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" ht="22" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="8" t="s">
@@ -2538,7 +2548,7 @@
     </row>
     <row r="85" spans="1:3" ht="22" customHeight="1">
       <c r="A85" s="6" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="8" t="s">
@@ -2547,7 +2557,7 @@
     </row>
     <row r="86" spans="1:3" ht="22" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="8" t="s">
@@ -2555,14 +2565,14 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="22" customHeight="1">
-      <c r="A87" s="10"/>
+      <c r="A87" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="B87" s="7"/>
       <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3" ht="22" customHeight="1">
-      <c r="A88" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="A88" s="10"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8" t="s">
         <v>39</v>
@@ -2570,7 +2580,7 @@
     </row>
     <row r="89" spans="1:3" ht="22" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="8" t="s">
@@ -2579,7 +2589,7 @@
     </row>
     <row r="90" spans="1:3" ht="22" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
@@ -2588,7 +2598,7 @@
     </row>
     <row r="91" spans="1:3" ht="22" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="8" t="s">
@@ -2597,7 +2607,7 @@
     </row>
     <row r="92" spans="1:3" ht="22" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="8" t="s">
@@ -2606,7 +2616,7 @@
     </row>
     <row r="93" spans="1:3" ht="22" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="8" t="s">
@@ -2615,7 +2625,7 @@
     </row>
     <row r="94" spans="1:3" ht="22" customHeight="1">
       <c r="A94" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
@@ -2624,7 +2634,7 @@
     </row>
     <row r="95" spans="1:3" ht="22" customHeight="1">
       <c r="A95" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="8" t="s">
@@ -2633,7 +2643,7 @@
     </row>
     <row r="96" spans="1:3" ht="22" customHeight="1">
       <c r="A96" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
@@ -2642,7 +2652,7 @@
     </row>
     <row r="97" spans="1:3" ht="22" customHeight="1">
       <c r="A97" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
@@ -2651,7 +2661,7 @@
     </row>
     <row r="98" spans="1:3" ht="22" customHeight="1">
       <c r="A98" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="8" t="s">
@@ -2660,7 +2670,7 @@
     </row>
     <row r="99" spans="1:3" ht="22" customHeight="1">
       <c r="A99" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="8" t="s">
@@ -2669,7 +2679,7 @@
     </row>
     <row r="100" spans="1:3" ht="22" customHeight="1">
       <c r="A100" s="6" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="8" t="s">
@@ -2678,7 +2688,7 @@
     </row>
     <row r="101" spans="1:3" ht="22" customHeight="1">
       <c r="A101" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="8" t="s">
@@ -2686,20 +2696,20 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="22" customHeight="1">
-      <c r="A102" s="10"/>
+      <c r="A102" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="B102" s="7"/>
       <c r="C102" s="9"/>
     </row>
     <row r="103" spans="1:3" ht="22" customHeight="1">
-      <c r="A103" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="A103" s="10"/>
       <c r="B103" s="7"/>
       <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" ht="22" customHeight="1">
       <c r="A104" s="6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="8" t="s">
@@ -2708,7 +2718,7 @@
     </row>
     <row r="105" spans="1:3" ht="22" customHeight="1">
       <c r="A105" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="8" t="s">
@@ -2717,7 +2727,7 @@
     </row>
     <row r="106" spans="1:3" ht="22" customHeight="1">
       <c r="A106" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="8" t="s">
@@ -2726,7 +2736,7 @@
     </row>
     <row r="107" spans="1:3" ht="22" customHeight="1">
       <c r="A107" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="8" t="s">
@@ -2735,7 +2745,7 @@
     </row>
     <row r="108" spans="1:3" ht="22" customHeight="1">
       <c r="A108" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108" s="7"/>
       <c r="C108" s="8" t="s">
@@ -2744,7 +2754,7 @@
     </row>
     <row r="109" spans="1:3" ht="22" customHeight="1">
       <c r="A109" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="8" t="s">
@@ -2752,20 +2762,20 @@
       </c>
     </row>
     <row r="110" spans="1:3" ht="22" customHeight="1">
-      <c r="A110" s="10"/>
+      <c r="A110" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="B110" s="7"/>
       <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3" ht="22" customHeight="1">
-      <c r="A111" s="6" t="s">
-        <v>106</v>
-      </c>
+      <c r="A111" s="10"/>
       <c r="B111" s="7"/>
       <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" ht="22" customHeight="1">
       <c r="A112" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B112" s="7"/>
       <c r="C112" s="8" t="s">
@@ -2774,7 +2784,7 @@
     </row>
     <row r="113" spans="1:3" ht="22" customHeight="1">
       <c r="A113" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B113" s="7"/>
       <c r="C113" s="8" t="s">
@@ -2782,20 +2792,20 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="22" customHeight="1">
-      <c r="A114" s="10"/>
+      <c r="A114" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="B114" s="7"/>
       <c r="C114" s="9"/>
     </row>
     <row r="115" spans="1:3" ht="22" customHeight="1">
-      <c r="A115" s="6" t="s">
-        <v>110</v>
-      </c>
+      <c r="A115" s="10"/>
       <c r="B115" s="7"/>
       <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" ht="22" customHeight="1">
       <c r="A116" s="6" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="B116" s="7"/>
       <c r="C116" s="8" t="s">
@@ -2803,20 +2813,20 @@
       </c>
     </row>
     <row r="117" spans="1:3" ht="22" customHeight="1">
-      <c r="A117" s="10"/>
+      <c r="A117" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="B117" s="7"/>
       <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" ht="22" customHeight="1">
-      <c r="A118" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="A118" s="10"/>
       <c r="B118" s="7"/>
       <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" ht="22" customHeight="1">
       <c r="A119" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B119" s="7"/>
       <c r="C119" s="8" t="s">
@@ -2825,7 +2835,7 @@
     </row>
     <row r="120" spans="1:3" ht="22" customHeight="1">
       <c r="A120" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B120" s="7"/>
       <c r="C120" s="8" t="s">
@@ -2833,20 +2843,20 @@
       </c>
     </row>
     <row r="121" spans="1:3" ht="22" customHeight="1">
-      <c r="A121" s="10"/>
+      <c r="A121" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="B121" s="7"/>
       <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" ht="22" customHeight="1">
-      <c r="A122" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="A122" s="10"/>
       <c r="B122" s="7"/>
       <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" ht="22" customHeight="1">
       <c r="A123" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B123" s="7"/>
       <c r="C123" s="8" t="s">
@@ -2854,20 +2864,20 @@
       </c>
     </row>
     <row r="124" spans="1:3" ht="22" customHeight="1">
-      <c r="A124" s="10"/>
+      <c r="A124" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="B124" s="7"/>
       <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" ht="22" customHeight="1">
-      <c r="A125" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="A125" s="10"/>
       <c r="B125" s="7"/>
       <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3" ht="22" customHeight="1">
       <c r="A126" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B126" s="7"/>
       <c r="C126" s="8" t="s">
@@ -2876,7 +2886,7 @@
     </row>
     <row r="127" spans="1:3" ht="22" customHeight="1">
       <c r="A127" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B127" s="7"/>
       <c r="C127" s="8" t="s">
@@ -2885,7 +2895,7 @@
     </row>
     <row r="128" spans="1:3" ht="22" customHeight="1">
       <c r="A128" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B128" s="7"/>
       <c r="C128" s="8" t="s">
@@ -2893,7 +2903,9 @@
       </c>
     </row>
     <row r="129" spans="1:3" ht="22" customHeight="1">
-      <c r="A129" s="10"/>
+      <c r="A129" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="B129" s="7"/>
       <c r="C129" s="9"/>
     </row>
@@ -3046,6 +3058,9 @@
       <c r="A159" s="10"/>
       <c r="B159" s="7"/>
       <c r="C159" s="9"/>
+    </row>
+    <row r="160" spans="1:3" ht="22" customHeight="1">
+      <c r="A160" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
fix unit of PT-INR
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fumiya/programming/medicaltest-to-text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD615F1-1F60-9D4D-B7A4-279AAB5106CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB4AE5-5163-864F-BA2D-C05C4154B847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="141">
   <si>
     <t>検査項目</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>APTT</t>
-  </si>
-  <si>
-    <t>sec</t>
   </si>
   <si>
     <t>D-dimer</t>
@@ -1882,7 +1879,7 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22" customHeight="1">
@@ -1936,7 +1933,7 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="22" customHeight="1">
@@ -1990,7 +1987,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="22" customHeight="1">
@@ -2025,11 +2022,11 @@
     </row>
     <row r="20" spans="1:3" ht="22" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="22" customHeight="1">
@@ -2044,9 +2041,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="22" customHeight="1">
       <c r="A23" s="6" t="s">
@@ -2054,12 +2049,12 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="22" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
@@ -2071,118 +2066,118 @@
     </row>
     <row r="26" spans="1:3" ht="22" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="22" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="22" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" ht="22" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="22" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="22" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="22" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="22" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="22" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="22" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="22" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="22" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="22" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="22" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
@@ -2191,7 +2186,7 @@
     </row>
     <row r="40" spans="1:3" ht="22" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
@@ -2200,7 +2195,7 @@
     </row>
     <row r="41" spans="1:3" ht="22" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
@@ -2209,174 +2204,174 @@
     </row>
     <row r="42" spans="1:3" ht="22" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" ht="22" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="22" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="22" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="22" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="22" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="22" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="22" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="22" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="22" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="22" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="22" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="22" customHeight="1">
       <c r="A54" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="22" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="22" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="22" customHeight="1">
       <c r="A57" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="22" customHeight="1">
       <c r="A58" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="22" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="22" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" ht="22" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="9"/>
@@ -2388,25 +2383,25 @@
     </row>
     <row r="63" spans="1:3" ht="22" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="22" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="22" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="9"/>
@@ -2418,7 +2413,7 @@
     </row>
     <row r="67" spans="1:3" ht="22" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="8" t="s">
@@ -2427,7 +2422,7 @@
     </row>
     <row r="68" spans="1:3" ht="22" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="8" t="s">
@@ -2436,7 +2431,7 @@
     </row>
     <row r="69" spans="1:3" ht="22" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="9"/>
@@ -2448,102 +2443,102 @@
     </row>
     <row r="71" spans="1:3" ht="22" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" ht="22" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" ht="22" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" ht="22" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" ht="22" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="22" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="22" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="22" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" ht="22" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="22" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" ht="22" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" ht="22" customHeight="1">
       <c r="A82" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" ht="22" customHeight="1">
       <c r="A83" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" ht="22" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="22" customHeight="1">
@@ -2552,7 +2547,7 @@
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="22" customHeight="1">
@@ -2561,12 +2556,12 @@
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="22" customHeight="1">
       <c r="A87" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="9"/>
@@ -2575,129 +2570,129 @@
       <c r="A88" s="10"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="22" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="22" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="22" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="22" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="22" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="22" customHeight="1">
       <c r="A94" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="22" customHeight="1">
       <c r="A95" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="22" customHeight="1">
       <c r="A96" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="22" customHeight="1">
       <c r="A97" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="22" customHeight="1">
       <c r="A98" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="22" customHeight="1">
       <c r="A99" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="22" customHeight="1">
       <c r="A100" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="22" customHeight="1">
       <c r="A101" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="22" customHeight="1">
       <c r="A102" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="9"/>
@@ -2709,61 +2704,61 @@
     </row>
     <row r="104" spans="1:3" ht="22" customHeight="1">
       <c r="A104" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="22" customHeight="1">
       <c r="A105" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="22" customHeight="1">
       <c r="A106" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="22" customHeight="1">
       <c r="A107" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="22" customHeight="1">
       <c r="A108" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B108" s="7"/>
       <c r="C108" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="22" customHeight="1">
       <c r="A109" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="22" customHeight="1">
       <c r="A110" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B110" s="7"/>
       <c r="C110" s="9"/>
@@ -2775,25 +2770,25 @@
     </row>
     <row r="112" spans="1:3" ht="22" customHeight="1">
       <c r="A112" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B112" s="7"/>
       <c r="C112" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="22" customHeight="1">
       <c r="A113" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B113" s="7"/>
       <c r="C113" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="22" customHeight="1">
       <c r="A114" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B114" s="7"/>
       <c r="C114" s="9"/>
@@ -2805,16 +2800,16 @@
     </row>
     <row r="116" spans="1:3" ht="22" customHeight="1">
       <c r="A116" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B116" s="7"/>
       <c r="C116" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="22" customHeight="1">
       <c r="A117" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B117" s="7"/>
       <c r="C117" s="9"/>
@@ -2826,25 +2821,25 @@
     </row>
     <row r="119" spans="1:3" ht="22" customHeight="1">
       <c r="A119" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B119" s="7"/>
       <c r="C119" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="22" customHeight="1">
       <c r="A120" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B120" s="7"/>
       <c r="C120" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="22" customHeight="1">
       <c r="A121" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B121" s="7"/>
       <c r="C121" s="9"/>
@@ -2856,16 +2851,16 @@
     </row>
     <row r="123" spans="1:3" ht="22" customHeight="1">
       <c r="A123" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B123" s="7"/>
       <c r="C123" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="22" customHeight="1">
       <c r="A124" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B124" s="7"/>
       <c r="C124" s="9"/>
@@ -2877,34 +2872,34 @@
     </row>
     <row r="126" spans="1:3" ht="22" customHeight="1">
       <c r="A126" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B126" s="7"/>
       <c r="C126" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="22" customHeight="1">
       <c r="A127" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B127" s="7"/>
       <c r="C127" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="22" customHeight="1">
       <c r="A128" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B128" s="7"/>
       <c r="C128" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="22" customHeight="1">
       <c r="A129" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B129" s="7"/>
       <c r="C129" s="9"/>

</xml_diff>

<commit_message>
add fibrinogen and blood type
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fumiya/programming/medicaltest-to-text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4238F052-9775-FF4E-B19A-887EFBFEC62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A88DC99-719F-CE47-9FC3-69371B6AF55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="145">
   <si>
     <t>検査項目</t>
   </si>
@@ -474,6 +474,37 @@
   </si>
   <si>
     <t>sec</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フィブリノーゲン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■血液型</t>
+    <rPh sb="1" eb="4">
+      <t xml:space="preserve">ケツエキガタ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABO式血液型</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">シキ </t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t xml:space="preserve">ケツエキガタ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rh式血液型</t>
+    <rPh sb="2" eb="3">
+      <t xml:space="preserve">シキ </t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ケツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1838,7 +1869,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2062,565 +2093,555 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="22" customHeight="1">
-      <c r="A25" s="10"/>
+      <c r="A25" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="22" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="22" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="22" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" ht="22" customHeight="1">
-      <c r="A29" s="6" t="s">
-        <v>32</v>
+      <c r="A29" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" ht="22" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A30" s="10"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" ht="22" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" s="7"/>
-      <c r="C31" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" ht="22" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="7"/>
-      <c r="C32" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="22" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B33" s="7"/>
-      <c r="C33" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" ht="22" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" ht="22" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="22" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="22" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="22" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>129</v>
+        <v>37</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="22" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="22" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="22" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="22" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="8" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="22" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="B43" s="7"/>
-      <c r="C43" s="9"/>
+      <c r="C43" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="22" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="22" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="8" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="22" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="8" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="22" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>132</v>
+        <v>45</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="22" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B48" s="7"/>
-      <c r="C48" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" ht="22" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="22" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="22" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="22" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="22" customHeight="1">
       <c r="A53" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="22" customHeight="1">
       <c r="A54" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="22" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="22" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="22" customHeight="1">
       <c r="A57" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="22" customHeight="1">
       <c r="A58" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="8" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="22" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="8" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="22" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="8" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="22" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="B61" s="7"/>
-      <c r="C61" s="9"/>
+      <c r="C61" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="22" customHeight="1">
-      <c r="A62" s="10"/>
+      <c r="A62" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="B62" s="7"/>
-      <c r="C62" s="9"/>
+      <c r="C62" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="63" spans="1:3" ht="22" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B63" s="7"/>
-      <c r="C63" s="9"/>
+      <c r="C63" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="22" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="22" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="22" customHeight="1">
-      <c r="A66" s="10"/>
+      <c r="A66" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="B66" s="7"/>
       <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" ht="22" customHeight="1">
-      <c r="A67" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="A67" s="10"/>
       <c r="B67" s="7"/>
       <c r="C67" s="9"/>
     </row>
     <row r="68" spans="1:3" ht="22" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="B68" s="7"/>
-      <c r="C68" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" ht="22" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="8" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="22" customHeight="1">
-      <c r="A70" s="10"/>
+      <c r="A70" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="B70" s="7"/>
-      <c r="C70" s="9"/>
+      <c r="C70" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="22" customHeight="1">
-      <c r="A71" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="A71" s="10"/>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" ht="22" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" ht="22" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="B73" s="7"/>
-      <c r="C73" s="9"/>
+      <c r="C73" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="74" spans="1:3" ht="22" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B74" s="7"/>
-      <c r="C74" s="9"/>
+      <c r="C74" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="22" customHeight="1">
-      <c r="A75" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="A75" s="10"/>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="22" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="22" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="22" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" ht="22" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="22" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" ht="22" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" ht="22" customHeight="1">
       <c r="A82" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" ht="22" customHeight="1">
       <c r="A83" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" ht="22" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" ht="22" customHeight="1">
       <c r="A85" s="6" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B85" s="7"/>
-      <c r="C85" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3" ht="22" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B86" s="7"/>
-      <c r="C86" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" ht="22" customHeight="1">
       <c r="A87" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B87" s="7"/>
-      <c r="C87" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3" ht="22" customHeight="1">
-      <c r="A88" s="10"/>
+      <c r="A88" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="B88" s="7"/>
       <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" ht="22" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B89" s="7"/>
-      <c r="C89" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:3" ht="22" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="8" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="22" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="8" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="22" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="8" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="22" customHeight="1">
-      <c r="A93" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="A93" s="10"/>
       <c r="B93" s="7"/>
-      <c r="C93" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" ht="22" customHeight="1">
       <c r="A94" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="8" t="s">
@@ -2629,52 +2650,52 @@
     </row>
     <row r="95" spans="1:3" ht="22" customHeight="1">
       <c r="A95" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="8" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="22" customHeight="1">
       <c r="A96" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="22" customHeight="1">
       <c r="A97" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="22" customHeight="1">
       <c r="A98" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="22" customHeight="1">
       <c r="A99" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="8" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="22" customHeight="1">
       <c r="A100" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="8" t="s">
@@ -2683,37 +2704,43 @@
     </row>
     <row r="101" spans="1:3" ht="22" customHeight="1">
       <c r="A101" s="6" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="8" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="22" customHeight="1">
       <c r="A102" s="6" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="8" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="22" customHeight="1">
-      <c r="A103" s="10"/>
+      <c r="A103" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="B103" s="7"/>
-      <c r="C103" s="9"/>
+      <c r="C103" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="22" customHeight="1">
       <c r="A104" s="6" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B104" s="7"/>
-      <c r="C104" s="9"/>
+      <c r="C104" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="105" spans="1:3" ht="22" customHeight="1">
       <c r="A105" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="8" t="s">
@@ -2722,188 +2749,188 @@
     </row>
     <row r="106" spans="1:3" ht="22" customHeight="1">
       <c r="A106" s="6" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="22" customHeight="1">
       <c r="A107" s="6" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="8" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="22" customHeight="1">
-      <c r="A108" s="6" t="s">
-        <v>101</v>
-      </c>
+      <c r="A108" s="10"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" ht="22" customHeight="1">
       <c r="A109" s="6" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="B109" s="7"/>
-      <c r="C109" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" ht="22" customHeight="1">
       <c r="A110" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B110" s="7"/>
       <c r="C110" s="8" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="22" customHeight="1">
-      <c r="A111" s="10"/>
+      <c r="A111" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="B111" s="7"/>
-      <c r="C111" s="9"/>
+      <c r="C111" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="22" customHeight="1">
       <c r="A112" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B112" s="7"/>
-      <c r="C112" s="9"/>
+      <c r="C112" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="113" spans="1:3" ht="22" customHeight="1">
       <c r="A113" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B113" s="7"/>
       <c r="C113" s="8" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="22" customHeight="1">
       <c r="A114" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B114" s="7"/>
       <c r="C114" s="8" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="22" customHeight="1">
-      <c r="A115" s="10"/>
+      <c r="A115" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="B115" s="7"/>
-      <c r="C115" s="9"/>
+      <c r="C115" s="8" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="116" spans="1:3" ht="22" customHeight="1">
-      <c r="A116" s="6" t="s">
-        <v>109</v>
-      </c>
+      <c r="A116" s="10"/>
       <c r="B116" s="7"/>
       <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" ht="22" customHeight="1">
       <c r="A117" s="6" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="B117" s="7"/>
-      <c r="C117" s="8" t="s">
+      <c r="C117" s="9"/>
+    </row>
+    <row r="118" spans="1:3" ht="22" customHeight="1">
+      <c r="A118" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B118" s="7"/>
+      <c r="C118" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="22" customHeight="1">
-      <c r="A118" s="10"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" ht="22" customHeight="1">
       <c r="A119" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B119" s="7"/>
-      <c r="C119" s="9"/>
+      <c r="C119" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="120" spans="1:3" ht="22" customHeight="1">
-      <c r="A120" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="A120" s="10"/>
       <c r="B120" s="7"/>
-      <c r="C120" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" ht="22" customHeight="1">
       <c r="A121" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B121" s="7"/>
-      <c r="C121" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" ht="22" customHeight="1">
-      <c r="A122" s="10"/>
+      <c r="A122" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="B122" s="7"/>
-      <c r="C122" s="9"/>
+      <c r="C122" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="123" spans="1:3" ht="22" customHeight="1">
-      <c r="A123" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="A123" s="10"/>
       <c r="B123" s="7"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" ht="22" customHeight="1">
       <c r="A124" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B124" s="7"/>
-      <c r="C124" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" ht="22" customHeight="1">
-      <c r="A125" s="10"/>
+      <c r="A125" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="B125" s="7"/>
-      <c r="C125" s="9"/>
+      <c r="C125" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="126" spans="1:3" ht="22" customHeight="1">
       <c r="A126" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B126" s="7"/>
-      <c r="C126" s="9"/>
+      <c r="C126" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="127" spans="1:3" ht="22" customHeight="1">
-      <c r="A127" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="A127" s="10"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" ht="22" customHeight="1">
       <c r="A128" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B128" s="7"/>
-      <c r="C128" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" ht="22" customHeight="1">
       <c r="A129" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B129" s="7"/>
       <c r="C129" s="8" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="22" customHeight="1">
@@ -2912,24 +2939,38 @@
       <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" ht="22" customHeight="1">
-      <c r="A131" s="10"/>
+      <c r="A131" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="B131" s="7"/>
       <c r="C131" s="9"/>
     </row>
     <row r="132" spans="1:3" ht="22" customHeight="1">
-      <c r="A132" s="10"/>
+      <c r="A132" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="B132" s="7"/>
-      <c r="C132" s="9"/>
+      <c r="C132" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="133" spans="1:3" ht="22" customHeight="1">
-      <c r="A133" s="10"/>
+      <c r="A133" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="B133" s="7"/>
-      <c r="C133" s="9"/>
+      <c r="C133" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="134" spans="1:3" ht="22" customHeight="1">
-      <c r="A134" s="10"/>
+      <c r="A134" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="B134" s="7"/>
-      <c r="C134" s="9"/>
+      <c r="C134" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="135" spans="1:3" ht="22" customHeight="1">
       <c r="A135" s="10"/>
@@ -3058,9 +3099,39 @@
     </row>
     <row r="160" spans="1:3" ht="22" customHeight="1">
       <c r="A160" s="10"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="9"/>
+    </row>
+    <row r="161" spans="1:3" ht="22" customHeight="1">
+      <c r="A161" s="10"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="9"/>
+    </row>
+    <row r="162" spans="1:3" ht="22" customHeight="1">
+      <c r="A162" s="10"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="9"/>
+    </row>
+    <row r="163" spans="1:3" ht="22" customHeight="1">
+      <c r="A163" s="10"/>
+      <c r="B163" s="7"/>
+      <c r="C163" s="9"/>
+    </row>
+    <row r="164" spans="1:3" ht="22" customHeight="1">
+      <c r="A164" s="10"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="9"/>
+    </row>
+    <row r="165" spans="1:3" ht="22" customHeight="1">
+      <c r="A165" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29" xr:uid="{03EACCED-FD89-434A-9090-C97F01B748E8}">
+      <formula1>"＋,−"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>

</xml_diff>